<commit_message>
Initial Conditions and Mapping
</commit_message>
<xml_diff>
--- a/scripts/datatools/IC/IC_From_DATA/Defaults_20130301.xlsx
+++ b/scripts/datatools/IC/IC_From_DATA/Defaults_20130301.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\datatools\IC\IC_From_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D979C4-4553-4D05-86EF-2CF7B6018BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E077F0-A92F-4835-ADCD-865A4CB798C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="2210" windowWidth="28800" windowHeight="15650"/>
+    <workbookView xWindow="8660" yWindow="2230" windowWidth="28800" windowHeight="15650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults_20130301" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Var</t>
   </si>
@@ -34,9 +44,6 @@
     <t>TRACE_1</t>
   </si>
   <si>
-    <t>WQ_TRC_AGE</t>
-  </si>
-  <si>
     <t>WQ_NCS_SS1</t>
   </si>
   <si>
@@ -83,13 +90,61 @@
   </si>
   <si>
     <t>WQ_DIAG_TOT_TP</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t>Zone 4</t>
+  </si>
+  <si>
+    <t>Zone 5</t>
+  </si>
+  <si>
+    <t>Zone 6</t>
+  </si>
+  <si>
+    <t>Zone 7</t>
+  </si>
+  <si>
+    <t>Zone 8</t>
+  </si>
+  <si>
+    <t>Zone 9</t>
+  </si>
+  <si>
+    <t>Zone 10</t>
+  </si>
+  <si>
+    <t>Zone 11</t>
+  </si>
+  <si>
+    <t>Zone 12</t>
+  </si>
+  <si>
+    <t>WQ_TRC_RET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +275,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -922,11 +983,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -938,132 +999,128 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B2">
-        <v>24.6157</v>
+        <v>0.3614</v>
       </c>
       <c r="C2">
-        <v>29.015699999999999</v>
+        <v>0.32879999999999998</v>
       </c>
       <c r="D2">
-        <v>36.28</v>
+        <v>0.32879999999999998</v>
       </c>
       <c r="E2">
-        <v>32.526600000000002</v>
+        <v>0.43409999999999999</v>
       </c>
       <c r="F2">
-        <v>26.323399999999999</v>
+        <v>0.23419999999999999</v>
       </c>
       <c r="G2">
-        <v>32.020400000000002</v>
+        <v>0.1678</v>
       </c>
       <c r="H2">
-        <f>(G2+I2)/2</f>
-        <v>38.745950000000001</v>
+        <v>0.1678</v>
       </c>
       <c r="I2">
-        <v>45.471499999999999</v>
+        <v>0.1678</v>
       </c>
       <c r="J2">
-        <v>64.200400000000002</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="K2">
-        <f>(J2+L2)/2</f>
-        <v>78.654899999999998</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="L2">
-        <v>93.109399999999994</v>
+        <v>-7.4800000000000005E-2</v>
       </c>
       <c r="M2">
-        <v>47.551000000000002</v>
+        <v>0.42180000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>21.621500000000001</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>21.052099999999999</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>20.62</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>20.864000000000001</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>21.365200000000002</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>21.039100000000001</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f>(G3+I3)/2</f>
-        <v>20.09205</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>19.145</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>20.223700000000001</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <f>(J3+L3)/2</f>
-        <v>20.576750000000001</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>20.9298</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>20.829899999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1104,741 +1161,869 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>24.6157</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>29.015699999999999</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>36.28</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>32.526600000000002</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>26.323399999999999</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>32.020400000000002</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <f>(G5+I5)/2</f>
+        <v>38.745950000000001</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>45.471499999999999</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>64.200400000000002</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <f>(J5+L5)/2</f>
+        <v>78.654899999999998</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>93.109399999999994</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>47.551000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>15.193099999999999</v>
+        <v>21.621500000000001</v>
       </c>
       <c r="C6">
-        <f>(B6+D6)/2</f>
-        <v>12.912749999999999</v>
+        <v>21.052099999999999</v>
       </c>
       <c r="D6">
-        <v>10.632400000000001</v>
+        <v>20.62</v>
       </c>
       <c r="E6">
-        <v>14.8462</v>
+        <v>20.864000000000001</v>
       </c>
       <c r="F6">
-        <v>12.750400000000001</v>
+        <v>21.365200000000002</v>
       </c>
       <c r="G6">
-        <v>13.790800000000001</v>
+        <v>21.039100000000001</v>
       </c>
       <c r="H6">
         <f>(G6+I6)/2</f>
-        <v>16.334800000000001</v>
+        <v>20.09205</v>
       </c>
       <c r="I6">
-        <v>18.878799999999998</v>
+        <v>19.145</v>
       </c>
       <c r="J6">
-        <v>21.8523</v>
+        <v>20.223700000000001</v>
       </c>
       <c r="K6">
         <f>(J6+L6)/2</f>
-        <v>21.358499999999999</v>
+        <v>20.576750000000001</v>
       </c>
       <c r="L6">
-        <v>20.864699999999999</v>
+        <v>20.9298</v>
       </c>
       <c r="M6">
-        <v>15.8942</v>
+        <v>20.829899999999999</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>249.11160000000001</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>159.93299999999999</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>228.375</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>206.9847</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>244.03909999999999</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>221.95310000000001</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f>(G7+I7)/2</f>
-        <v>207.73435000000001</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>193.51560000000001</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>226.01560000000001</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <f>(J7+L7)/2</f>
-        <v>193.16405</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>160.3125</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>158.5521</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>68.208799999999997</v>
+        <v>15.193099999999999</v>
       </c>
       <c r="C8">
         <f>(B8+D8)/2</f>
-        <v>47.471849999999996</v>
+        <v>12.912749999999999</v>
       </c>
       <c r="D8">
-        <v>26.7349</v>
+        <v>10.632400000000001</v>
       </c>
       <c r="E8">
-        <v>103.2028</v>
+        <v>14.8462</v>
       </c>
       <c r="F8">
-        <v>152.9359</v>
+        <v>12.750400000000001</v>
       </c>
       <c r="G8">
-        <v>152.9359</v>
+        <v>13.790800000000001</v>
       </c>
       <c r="H8">
-        <v>152.9359</v>
+        <f>(G8+I8)/2</f>
+        <v>16.334800000000001</v>
       </c>
       <c r="I8">
-        <v>152.9359</v>
+        <v>18.878799999999998</v>
       </c>
       <c r="J8">
-        <v>128.57140000000001</v>
+        <v>21.8523</v>
       </c>
       <c r="K8">
-        <v>128.57140000000001</v>
+        <f>(J8+L8)/2</f>
+        <v>21.358499999999999</v>
       </c>
       <c r="L8">
-        <v>128.57140000000001</v>
+        <v>20.864699999999999</v>
       </c>
       <c r="M8">
-        <v>128.57140000000001</v>
+        <v>15.8942</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>1.2023999999999999</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <f>(B9+D9)/2</f>
-        <v>0.77974999999999994</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.35709999999999997</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1.5713999999999999</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.39290000000000003</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.39290000000000003</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.39290000000000003</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.39290000000000003</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0.35709999999999997</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0.35709999999999997</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0.35709999999999997</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>0.35709999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>0.27379999999999999</v>
+        <v>249.11160000000001</v>
       </c>
       <c r="C10">
-        <f>(B10+D10)/2</f>
-        <v>0.24404999999999999</v>
+        <v>159.93299999999999</v>
       </c>
       <c r="D10">
-        <v>0.21429999999999999</v>
+        <v>228.375</v>
       </c>
       <c r="E10">
-        <v>1.25</v>
+        <v>206.9847</v>
       </c>
       <c r="F10">
-        <v>0.21429999999999999</v>
+        <v>244.03909999999999</v>
       </c>
       <c r="G10">
-        <v>0.21429999999999999</v>
+        <v>221.95310000000001</v>
       </c>
       <c r="H10">
-        <v>0.21429999999999999</v>
+        <f>(G10+I10)/2</f>
+        <v>207.73435000000001</v>
       </c>
       <c r="I10">
-        <v>0.21429999999999999</v>
+        <v>193.51560000000001</v>
       </c>
       <c r="J10">
-        <v>0.21429999999999999</v>
+        <v>226.01560000000001</v>
       </c>
       <c r="K10">
-        <v>0.21429999999999999</v>
+        <f>(J10+L10)/2</f>
+        <v>193.16405</v>
       </c>
       <c r="L10">
-        <v>0.21429999999999999</v>
+        <v>160.3125</v>
       </c>
       <c r="M10">
-        <v>0.21429999999999999</v>
+        <v>158.5521</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>0.18279999999999999</v>
+        <v>68.208799999999997</v>
       </c>
       <c r="C11">
         <f>(B11+D11)/2</f>
-        <v>0.30914999999999998</v>
+        <v>47.471849999999996</v>
       </c>
       <c r="D11">
-        <v>0.4355</v>
+        <v>26.7349</v>
       </c>
       <c r="E11">
-        <v>0.4355</v>
+        <v>103.2028</v>
       </c>
       <c r="F11">
-        <v>0.1452</v>
+        <v>152.9359</v>
       </c>
       <c r="G11">
-        <v>0.1452</v>
+        <v>152.9359</v>
       </c>
       <c r="H11">
-        <v>0.1452</v>
+        <v>152.9359</v>
       </c>
       <c r="I11">
-        <v>0.1452</v>
+        <v>152.9359</v>
       </c>
       <c r="J11">
-        <v>0.1613</v>
+        <v>128.57140000000001</v>
       </c>
       <c r="K11">
-        <v>0.1613</v>
+        <v>128.57140000000001</v>
       </c>
       <c r="L11">
-        <v>0.1613</v>
+        <v>128.57140000000001</v>
       </c>
       <c r="M11">
-        <v>0.1613</v>
+        <v>128.57140000000001</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>1.83E-2</v>
+        <v>1.2023999999999999</v>
       </c>
       <c r="C12">
         <f>(B12+D12)/2</f>
-        <v>3.0899999999999997E-2</v>
+        <v>0.77974999999999994</v>
       </c>
       <c r="D12">
-        <v>4.3499999999999997E-2</v>
+        <v>0.35709999999999997</v>
       </c>
       <c r="E12">
-        <v>4.3499999999999997E-2</v>
+        <v>1.5713999999999999</v>
       </c>
       <c r="F12">
-        <v>1.4500000000000001E-2</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="G12">
-        <v>1.4500000000000001E-2</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="H12">
-        <v>1.4500000000000001E-2</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="I12">
-        <v>1.4500000000000001E-2</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="J12">
-        <v>1.61E-2</v>
+        <v>0.35709999999999997</v>
       </c>
       <c r="K12">
-        <v>1.61E-2</v>
+        <v>0.35709999999999997</v>
       </c>
       <c r="L12">
-        <v>1.61E-2</v>
+        <v>0.35709999999999997</v>
       </c>
       <c r="M12">
-        <v>1.61E-2</v>
+        <v>0.35709999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>716.66669999999999</v>
+        <v>0.27379999999999999</v>
       </c>
       <c r="C13">
-        <v>716.66669999999999</v>
+        <f>(B13+D13)/2</f>
+        <v>0.24404999999999999</v>
       </c>
       <c r="D13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="E13">
-        <v>716.66669999999999</v>
+        <v>1.25</v>
       </c>
       <c r="F13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="G13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="H13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="I13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="J13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="K13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="L13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
       <c r="M13">
-        <v>716.66669999999999</v>
+        <v>0.21429999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>718.11710000000005</v>
+        <v>0.18279999999999999</v>
       </c>
       <c r="C14">
-        <v>718.11710000000005</v>
+        <f>(B14+D14)/2</f>
+        <v>0.30914999999999998</v>
       </c>
       <c r="D14">
-        <v>718.11710000000005</v>
+        <v>0.4355</v>
       </c>
       <c r="E14">
-        <v>718.11710000000005</v>
+        <v>0.4355</v>
       </c>
       <c r="F14">
-        <v>718.11710000000005</v>
+        <v>0.1452</v>
       </c>
       <c r="G14">
-        <v>718.11710000000005</v>
+        <v>0.1452</v>
       </c>
       <c r="H14">
-        <v>718.11710000000005</v>
+        <v>0.1452</v>
       </c>
       <c r="I14">
-        <v>718.11710000000005</v>
+        <v>0.1452</v>
       </c>
       <c r="J14">
-        <v>718.11710000000005</v>
+        <v>0.1613</v>
       </c>
       <c r="K14">
-        <v>718.11710000000005</v>
+        <v>0.1613</v>
       </c>
       <c r="L14">
-        <v>718.11710000000005</v>
+        <v>0.1613</v>
       </c>
       <c r="M14">
-        <v>718.11710000000005</v>
+        <v>0.1613</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15">
+        <v>1.83E-2</v>
+      </c>
+      <c r="C15">
+        <f>(B15+D15)/2</f>
+        <v>3.0899999999999997E-2</v>
+      </c>
+      <c r="D15">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="E15">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F15">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="J15">
+        <v>1.61E-2</v>
+      </c>
+      <c r="K15">
+        <v>1.61E-2</v>
+      </c>
+      <c r="L15">
+        <v>1.61E-2</v>
+      </c>
+      <c r="M15">
+        <v>1.61E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="C16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="D16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="E16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="F16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="G16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="H16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="I16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="J16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="K16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="L16">
+        <v>716.66669999999999</v>
+      </c>
+      <c r="M16">
+        <v>716.66669999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="C17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="D17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="E17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="F17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="G17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="H17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="I17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="J17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="K17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="L17">
+        <v>718.11710000000005</v>
+      </c>
+      <c r="M17">
+        <v>718.11710000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
         <v>50.179699999999997</v>
       </c>
-      <c r="C15">
-        <f>(C20-C9-C10)/2</f>
+      <c r="C18">
+        <f>(C23-C12-C13)/2</f>
         <v>27.34525</v>
       </c>
-      <c r="D15">
-        <f t="shared" ref="D15:L15" si="0">(D20-D9-D10)/2</f>
+      <c r="D18">
+        <f t="shared" ref="D18:L18" si="0">(D23-D12-D13)/2</f>
         <v>15.785749999999998</v>
       </c>
-      <c r="E15">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>35.375</v>
       </c>
-      <c r="F15">
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>19.696400000000001</v>
       </c>
-      <c r="G15">
+      <c r="G18">
         <f t="shared" si="0"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="H15">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="I15">
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="J15">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>139</v>
       </c>
-      <c r="K15">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>137.928575</v>
       </c>
-      <c r="L15">
+      <c r="L18">
         <f t="shared" si="0"/>
         <v>136.85715000000002</v>
       </c>
-      <c r="M15">
+      <c r="M18">
         <v>60.208300000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f>B15</f>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <f>B18</f>
         <v>50.179699999999997</v>
       </c>
-      <c r="C16">
-        <f>C15</f>
+      <c r="C19">
+        <f>C18</f>
         <v>27.34525</v>
       </c>
-      <c r="D16">
-        <f t="shared" ref="D16:L16" si="1">D15</f>
+      <c r="D19">
+        <f t="shared" ref="D19:L19" si="1">D18</f>
         <v>15.785749999999998</v>
       </c>
-      <c r="E16">
+      <c r="E19">
         <f t="shared" si="1"/>
         <v>35.375</v>
       </c>
-      <c r="F16">
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>19.696400000000001</v>
       </c>
-      <c r="G16">
+      <c r="G19">
         <f t="shared" si="1"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="H16">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="I16">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>33.267850000000003</v>
       </c>
-      <c r="J16">
+      <c r="J19">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="K16">
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>137.928575</v>
       </c>
-      <c r="L16">
+      <c r="L19">
         <f t="shared" si="1"/>
         <v>136.85715000000002</v>
       </c>
-      <c r="M16">
+      <c r="M19">
         <v>60.208300000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.87239999999999995</v>
-      </c>
-      <c r="C17">
-        <f>(B17+D17)/2</f>
-        <v>0.62004999999999999</v>
-      </c>
-      <c r="D17">
-        <v>0.36770000000000003</v>
-      </c>
-      <c r="E17">
-        <v>0.95940000000000003</v>
-      </c>
-      <c r="F17">
-        <v>1.1192</v>
-      </c>
-      <c r="G17">
-        <v>1.1192</v>
-      </c>
-      <c r="H17">
-        <v>1.1192</v>
-      </c>
-      <c r="I17">
-        <v>1.1192</v>
-      </c>
-      <c r="J17">
-        <v>3.8887999999999998</v>
-      </c>
-      <c r="K17">
-        <v>3.8887999999999998</v>
-      </c>
-      <c r="L17">
-        <v>3.8887999999999998</v>
-      </c>
-      <c r="M17">
-        <v>3.8887999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1.0905</v>
-      </c>
-      <c r="C18">
-        <f>(B18+D18)/2</f>
-        <v>0.77505000000000002</v>
-      </c>
-      <c r="D18">
-        <v>0.45960000000000001</v>
-      </c>
-      <c r="E18">
-        <v>1.1992</v>
-      </c>
-      <c r="F18">
-        <v>1.399</v>
-      </c>
-      <c r="G18">
-        <v>1.399</v>
-      </c>
-      <c r="H18">
-        <v>1.399</v>
-      </c>
-      <c r="I18">
-        <v>1.399</v>
-      </c>
-      <c r="J18">
-        <v>4.8609999999999998</v>
-      </c>
-      <c r="K18">
-        <v>4.8609999999999998</v>
-      </c>
-      <c r="L18">
-        <v>4.8609999999999998</v>
-      </c>
-      <c r="M18">
-        <v>4.8609999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>24.229199999999999</v>
-      </c>
-      <c r="C19">
-        <f>(B19+D19)/2</f>
-        <v>24.229199999999999</v>
-      </c>
-      <c r="D19">
-        <v>24.229199999999999</v>
-      </c>
-      <c r="E19">
-        <f>(D19+F19)/2</f>
-        <v>58.572950000000006</v>
-      </c>
-      <c r="F19">
-        <v>92.916700000000006</v>
-      </c>
-      <c r="G19">
-        <v>92.916700000000006</v>
-      </c>
-      <c r="H19">
-        <v>92.916700000000006</v>
-      </c>
-      <c r="I19">
-        <v>92.916700000000006</v>
-      </c>
-      <c r="J19">
-        <v>112.6482</v>
-      </c>
-      <c r="K19">
-        <v>112.6482</v>
-      </c>
-      <c r="L19">
-        <v>112.6482</v>
-      </c>
-      <c r="M19">
-        <v>112.6482</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>79.285700000000006</v>
+        <v>0.87239999999999995</v>
       </c>
       <c r="C20">
         <f>(B20+D20)/2</f>
-        <v>55.714300000000001</v>
+        <v>0.62004999999999999</v>
       </c>
       <c r="D20">
-        <v>32.142899999999997</v>
+        <v>0.36770000000000003</v>
       </c>
       <c r="E20">
-        <v>73.571399999999997</v>
+        <v>0.95940000000000003</v>
       </c>
       <c r="F20">
-        <v>40</v>
+        <v>1.1192</v>
       </c>
       <c r="G20">
-        <v>67.142899999999997</v>
+        <v>1.1192</v>
       </c>
       <c r="H20">
-        <v>67.142899999999997</v>
+        <v>1.1192</v>
       </c>
       <c r="I20">
-        <v>67.142899999999997</v>
+        <v>1.1192</v>
       </c>
       <c r="J20">
-        <v>278.57139999999998</v>
+        <v>3.8887999999999998</v>
       </c>
       <c r="K20">
-        <f>(J20+L20)/2</f>
-        <v>276.42854999999997</v>
+        <v>3.8887999999999998</v>
       </c>
       <c r="L20">
-        <v>274.28570000000002</v>
+        <v>3.8887999999999998</v>
       </c>
       <c r="M20">
-        <v>271.42860000000002</v>
+        <v>3.8887999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>2.5806</v>
+        <v>1.0905</v>
       </c>
       <c r="C21">
         <f>(B21+D21)/2</f>
+        <v>0.77505000000000002</v>
+      </c>
+      <c r="D21">
+        <v>0.45960000000000001</v>
+      </c>
+      <c r="E21">
+        <v>1.1992</v>
+      </c>
+      <c r="F21">
+        <v>1.399</v>
+      </c>
+      <c r="G21">
+        <v>1.399</v>
+      </c>
+      <c r="H21">
+        <v>1.399</v>
+      </c>
+      <c r="I21">
+        <v>1.399</v>
+      </c>
+      <c r="J21">
+        <v>4.8609999999999998</v>
+      </c>
+      <c r="K21">
+        <v>4.8609999999999998</v>
+      </c>
+      <c r="L21">
+        <v>4.8609999999999998</v>
+      </c>
+      <c r="M21">
+        <v>4.8609999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>24.229199999999999</v>
+      </c>
+      <c r="C22">
+        <f>(B22+D22)/2</f>
+        <v>24.229199999999999</v>
+      </c>
+      <c r="D22">
+        <v>24.229199999999999</v>
+      </c>
+      <c r="E22">
+        <f>(D22+F22)/2</f>
+        <v>58.572950000000006</v>
+      </c>
+      <c r="F22">
+        <v>92.916700000000006</v>
+      </c>
+      <c r="G22">
+        <v>92.916700000000006</v>
+      </c>
+      <c r="H22">
+        <v>92.916700000000006</v>
+      </c>
+      <c r="I22">
+        <v>92.916700000000006</v>
+      </c>
+      <c r="J22">
+        <v>112.6482</v>
+      </c>
+      <c r="K22">
+        <v>112.6482</v>
+      </c>
+      <c r="L22">
+        <v>112.6482</v>
+      </c>
+      <c r="M22">
+        <v>112.6482</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>79.285700000000006</v>
+      </c>
+      <c r="C23">
+        <f>(B23+D23)/2</f>
+        <v>55.714300000000001</v>
+      </c>
+      <c r="D23">
+        <v>32.142899999999997</v>
+      </c>
+      <c r="E23">
+        <v>73.571399999999997</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23">
+        <v>67.142899999999997</v>
+      </c>
+      <c r="H23">
+        <v>67.142899999999997</v>
+      </c>
+      <c r="I23">
+        <v>67.142899999999997</v>
+      </c>
+      <c r="J23">
+        <v>278.57139999999998</v>
+      </c>
+      <c r="K23">
+        <f>(J23+L23)/2</f>
+        <v>276.42854999999997</v>
+      </c>
+      <c r="L23">
+        <v>274.28570000000002</v>
+      </c>
+      <c r="M23">
+        <v>271.42860000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>2.5806</v>
+      </c>
+      <c r="C24">
+        <f>(B24+D24)/2</f>
         <v>1.9677</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>1.3548</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>3</v>
       </c>
-      <c r="F21">
+      <c r="F24">
         <v>1.5484</v>
       </c>
-      <c r="G21">
+      <c r="G24">
         <v>2.0968</v>
       </c>
-      <c r="H21">
+      <c r="H24">
         <v>2.0968</v>
       </c>
-      <c r="I21">
+      <c r="I24">
         <v>2.0968</v>
       </c>
-      <c r="J21">
+      <c r="J24">
         <v>9.0968</v>
       </c>
-      <c r="K21">
-        <f>(J21+L21)/2</f>
+      <c r="K24">
+        <f>(J24+L24)/2</f>
         <v>9.0806500000000003</v>
       </c>
-      <c r="L21">
+      <c r="L24">
         <v>9.0645000000000007</v>
       </c>
-      <c r="M21">
+      <c r="M24">
         <v>7.5805999999999996</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>